<commit_message>
Update UPPERCASE letters in invoice
</commit_message>
<xml_diff>
--- a/main/catalogue/DATA SETUP.xlsx
+++ b/main/catalogue/DATA SETUP.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cypherjac.CYPHERJAC\Desktop\Projects\catalogue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\catalogue_app\main\catalogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F2D7BE-F12E-4AE7-B858-565AA5100E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="2"/>
+    <workbookView xWindow="870" yWindow="0" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WAREHOUSES" sheetId="7" r:id="rId1"/>
@@ -18,13 +19,14 @@
     <sheet name="BUYERS" sheetId="3" r:id="rId4"/>
     <sheet name="TEA GRADES" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4235,7 +4237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5107,6 +5109,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5142,6 +5161,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5317,26 +5353,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J95"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="64" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="46.44140625" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="61.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="61.85546875" customWidth="1"/>
     <col min="8" max="8" width="67" customWidth="1"/>
-    <col min="9" max="9" width="37.33203125" customWidth="1"/>
+    <col min="9" max="9" width="37.28515625" customWidth="1"/>
     <col min="10" max="10" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="148" t="s">
         <v>713</v>
       </c>
@@ -5348,7 +5384,7 @@
       <c r="I1" s="148"/>
       <c r="J1" s="148"/>
     </row>
-    <row r="2" spans="3:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="112" t="s">
         <v>693</v>
       </c>
@@ -5371,7 +5407,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="3" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="56">
         <v>1</v>
       </c>
@@ -5395,7 +5431,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="3:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
         <v>392</v>
@@ -5411,7 +5447,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="3:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
         <v>394</v>
@@ -5427,7 +5463,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
         <v>392</v>
@@ -5439,7 +5475,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -5463,7 +5499,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
       <c r="D8" s="4" t="s">
         <v>398</v>
@@ -5477,7 +5513,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="4" t="s">
         <v>400</v>
@@ -5491,7 +5527,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3">
         <v>3</v>
       </c>
@@ -5513,7 +5549,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
         <v>1010</v>
@@ -5527,7 +5563,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3">
         <v>4</v>
       </c>
@@ -5553,7 +5589,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="4" t="s">
         <v>714</v>
@@ -5567,7 +5603,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="4" t="s">
         <v>404</v>
@@ -5581,7 +5617,7 @@
       <c r="I14" s="7"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
         <v>406</v>
@@ -5595,7 +5631,7 @@
       <c r="I15" s="7"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
       <c r="D16" s="4" t="s">
         <v>408</v>
@@ -5609,7 +5645,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
         <v>410</v>
@@ -5623,7 +5659,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
       <c r="D18" s="4" t="s">
         <v>412</v>
@@ -5637,7 +5673,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
       <c r="D19" s="4" t="s">
         <v>414</v>
@@ -5651,7 +5687,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="4" t="s">
         <v>416</v>
@@ -5665,7 +5701,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -5689,7 +5725,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
       <c r="D22" s="6" t="s">
         <v>419</v>
@@ -5703,7 +5739,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="6" t="s">
         <v>421</v>
@@ -5717,7 +5753,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
       <c r="D24" s="6" t="s">
         <v>423</v>
@@ -5731,7 +5767,7 @@
       <c r="I24" s="7"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
       <c r="D25" s="6" t="s">
         <v>425</v>
@@ -5745,7 +5781,7 @@
       <c r="I25" s="7"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="6" t="s">
         <v>462</v>
@@ -5759,7 +5795,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="6" t="s">
         <v>686</v>
@@ -5773,7 +5809,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
       <c r="D28" s="6" t="s">
         <v>427</v>
@@ -5787,7 +5823,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
       <c r="D29" s="6" t="s">
         <v>715</v>
@@ -5801,7 +5837,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="66"/>
       <c r="D30" s="67" t="s">
         <v>727</v>
@@ -5815,7 +5851,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="66"/>
       <c r="D31" s="71" t="s">
         <v>729</v>
@@ -5829,7 +5865,7 @@
       <c r="I31" s="7"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="66"/>
       <c r="D32" s="71" t="s">
         <v>922</v>
@@ -5843,7 +5879,7 @@
       <c r="I32" s="7"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="66"/>
       <c r="D33" s="71" t="s">
         <v>929</v>
@@ -5857,7 +5893,7 @@
       <c r="I33" s="7"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="66">
         <v>6</v>
       </c>
@@ -5881,7 +5917,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="66"/>
       <c r="D35" s="71" t="s">
         <v>967</v>
@@ -5895,7 +5931,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="66">
         <v>7</v>
       </c>
@@ -5921,7 +5957,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="37" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="3">
         <v>8</v>
       </c>
@@ -5945,7 +5981,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="3"/>
       <c r="D38" s="4" t="s">
         <v>490</v>
@@ -5959,7 +5995,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="4" t="s">
         <v>491</v>
@@ -5973,7 +6009,7 @@
       <c r="I39" s="7"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="4" t="s">
         <v>492</v>
@@ -5987,7 +6023,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="4" t="s">
         <v>493</v>
@@ -6001,7 +6037,7 @@
       <c r="I41" s="7"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="4" t="s">
         <v>494</v>
@@ -6015,7 +6051,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
       <c r="D43" s="4" t="s">
         <v>495</v>
@@ -6029,7 +6065,7 @@
       <c r="I43" s="7"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
       <c r="D44" s="4" t="s">
         <v>496</v>
@@ -6043,7 +6079,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
       <c r="D45" s="4" t="s">
         <v>497</v>
@@ -6057,7 +6093,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="3">
         <v>9</v>
       </c>
@@ -6081,7 +6117,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="47" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
       <c r="D47" s="4" t="s">
         <v>882</v>
@@ -6095,7 +6131,7 @@
       <c r="I47" s="7"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="3"/>
       <c r="D48" s="4" t="s">
         <v>931</v>
@@ -6109,7 +6145,7 @@
       <c r="I48" s="7"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="3">
         <v>10</v>
       </c>
@@ -6133,7 +6169,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="3"/>
       <c r="D50" s="4" t="s">
         <v>434</v>
@@ -6147,7 +6183,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="4" t="s">
         <v>436</v>
@@ -6161,7 +6197,7 @@
       <c r="I51" s="7"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="3"/>
       <c r="D52" s="4" t="s">
         <v>594</v>
@@ -6175,7 +6211,7 @@
       <c r="I52" s="7"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="3:10" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:10" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="3"/>
       <c r="D53" s="72" t="s">
         <v>1016</v>
@@ -6189,7 +6225,7 @@
       <c r="I53" s="7"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="3:10" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:10" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="3"/>
       <c r="D54" s="72" t="s">
         <v>734</v>
@@ -6203,7 +6239,7 @@
       <c r="I54" s="7"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
       <c r="D55" s="74" t="s">
         <v>1017</v>
@@ -6217,7 +6253,7 @@
       <c r="I55" s="7"/>
       <c r="J55" s="8"/>
     </row>
-    <row r="56" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="3"/>
       <c r="D56" s="23" t="s">
         <v>781</v>
@@ -6231,7 +6267,7 @@
       <c r="I56" s="7"/>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="3"/>
       <c r="D57" s="23" t="s">
         <v>925</v>
@@ -6245,7 +6281,7 @@
       <c r="I57" s="7"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="75" t="s">
         <v>1019</v>
@@ -6259,7 +6295,7 @@
       <c r="I58" s="7"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="3"/>
       <c r="D59" s="75" t="s">
         <v>1296</v>
@@ -6273,7 +6309,7 @@
       <c r="I59" s="7"/>
       <c r="J59" s="8"/>
     </row>
-    <row r="60" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="3">
         <v>11</v>
       </c>
@@ -6295,7 +6331,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="61" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="3"/>
       <c r="D61" s="75" t="s">
         <v>1103</v>
@@ -6309,7 +6345,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="8"/>
     </row>
-    <row r="62" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="3">
         <v>12</v>
       </c>
@@ -6331,7 +6367,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="63" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="75" t="s">
         <v>1133</v>
@@ -6345,7 +6381,7 @@
       <c r="I63" s="7"/>
       <c r="J63" s="8"/>
     </row>
-    <row r="64" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="3">
         <v>13</v>
       </c>
@@ -6369,7 +6405,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="65" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="3"/>
       <c r="D65" s="4" t="s">
         <v>988</v>
@@ -6385,7 +6421,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="66" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="3"/>
       <c r="D66" s="4" t="s">
         <v>1293</v>
@@ -6401,7 +6437,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="67" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="3">
         <v>14</v>
       </c>
@@ -6425,7 +6461,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="68" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="3"/>
       <c r="D68" s="4" t="s">
         <v>915</v>
@@ -6441,7 +6477,7 @@
       <c r="I68" s="7"/>
       <c r="J68" s="8"/>
     </row>
-    <row r="69" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="3"/>
       <c r="D69" s="4" t="s">
         <v>916</v>
@@ -6457,7 +6493,7 @@
       <c r="I69" s="7"/>
       <c r="J69" s="8"/>
     </row>
-    <row r="70" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="3"/>
       <c r="D70" s="4" t="s">
         <v>918</v>
@@ -6473,7 +6509,7 @@
       <c r="I70" s="7"/>
       <c r="J70" s="8"/>
     </row>
-    <row r="71" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="3"/>
       <c r="D71" s="4" t="s">
         <v>947</v>
@@ -6489,7 +6525,7 @@
       <c r="I71" s="7"/>
       <c r="J71" s="8"/>
     </row>
-    <row r="72" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="3"/>
       <c r="D72" s="4" t="s">
         <v>1140</v>
@@ -6503,7 +6539,7 @@
       <c r="I72" s="7"/>
       <c r="J72" s="8"/>
     </row>
-    <row r="73" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="3"/>
       <c r="D73" s="4" t="s">
         <v>1145</v>
@@ -6517,7 +6553,7 @@
       <c r="I73" s="7"/>
       <c r="J73" s="8"/>
     </row>
-    <row r="74" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="3">
         <v>15</v>
       </c>
@@ -6543,7 +6579,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="75" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="9"/>
       <c r="D75" s="4" t="s">
         <v>1227</v>
@@ -6557,7 +6593,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="8"/>
     </row>
-    <row r="76" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="3"/>
       <c r="D76" s="4" t="s">
         <v>1228</v>
@@ -6571,7 +6607,7 @@
       <c r="I76" s="7"/>
       <c r="J76" s="8"/>
     </row>
-    <row r="77" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="3">
         <v>16</v>
       </c>
@@ -6595,7 +6631,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="78" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="3"/>
       <c r="D78" s="4" t="s">
         <v>449</v>
@@ -6609,7 +6645,7 @@
       <c r="I78" s="7"/>
       <c r="J78" s="8"/>
     </row>
-    <row r="79" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="3"/>
       <c r="D79" s="4" t="s">
         <v>451</v>
@@ -6623,7 +6659,7 @@
       <c r="I79" s="7"/>
       <c r="J79" s="8"/>
     </row>
-    <row r="80" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="3">
         <v>17</v>
       </c>
@@ -6649,7 +6685,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="81" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="3"/>
       <c r="D81" s="4" t="s">
         <v>456</v>
@@ -6663,7 +6699,7 @@
       <c r="I81" s="7"/>
       <c r="J81" s="8"/>
     </row>
-    <row r="82" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="3"/>
       <c r="D82" s="4" t="s">
         <v>458</v>
@@ -6677,7 +6713,7 @@
       <c r="I82" s="7"/>
       <c r="J82" s="8"/>
     </row>
-    <row r="84" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C84" s="148" t="s">
         <v>1326</v>
       </c>
@@ -6689,7 +6725,7 @@
       <c r="I84" s="148"/>
       <c r="J84" s="148"/>
     </row>
-    <row r="85" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D85" s="112" t="s">
         <v>693</v>
       </c>
@@ -6712,7 +6748,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="86" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="81"/>
       <c r="C86" s="3">
         <v>18</v>
@@ -6737,7 +6773,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="87" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="C87" s="3">
         <v>19</v>
@@ -6762,7 +6798,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="C88" s="3">
         <v>20</v>
@@ -6789,7 +6825,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="89" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="C89" s="3">
         <v>21</v>
@@ -6812,7 +6848,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="90" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
       <c r="C90" s="3">
         <v>22</v>
@@ -6837,7 +6873,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="91" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
       <c r="C91" s="3">
         <v>23</v>
@@ -6860,7 +6896,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="92" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
       <c r="C92" s="3">
         <v>24</v>
@@ -6887,7 +6923,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="93" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="3">
         <v>25</v>
@@ -6912,7 +6948,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="94" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
       <c r="C94" s="3">
         <v>26</v>
@@ -6939,7 +6975,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="95" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
       <c r="C95" s="3">
         <v>27</v>
@@ -6970,56 +7006,56 @@
     <mergeCell ref="C84:J84"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J12" r:id="rId1"/>
-    <hyperlink ref="J49" r:id="rId2"/>
-    <hyperlink ref="J74" r:id="rId3"/>
-    <hyperlink ref="J3" r:id="rId4"/>
-    <hyperlink ref="J77" r:id="rId5"/>
-    <hyperlink ref="J80" r:id="rId6"/>
-    <hyperlink ref="J64" r:id="rId7"/>
-    <hyperlink ref="J65" r:id="rId8"/>
-    <hyperlink ref="J21" r:id="rId9"/>
-    <hyperlink ref="J67" r:id="rId10"/>
-    <hyperlink ref="J7" r:id="rId11"/>
-    <hyperlink ref="J37" r:id="rId12"/>
-    <hyperlink ref="J36" r:id="rId13"/>
-    <hyperlink ref="J46" r:id="rId14"/>
-    <hyperlink ref="J34" r:id="rId15"/>
-    <hyperlink ref="J10" r:id="rId16"/>
-    <hyperlink ref="J62" r:id="rId17"/>
-    <hyperlink ref="J66" r:id="rId18"/>
-    <hyperlink ref="J87" r:id="rId19"/>
-    <hyperlink ref="J90" r:id="rId20"/>
-    <hyperlink ref="J91" r:id="rId21" display="mailto:ALKHALIFAENTERPRISES@gmail.com"/>
-    <hyperlink ref="J94" r:id="rId22"/>
+    <hyperlink ref="J12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J49" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J74" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J77" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J80" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J64" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J65" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J67" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J46" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J34" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J62" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J66" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J87" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J90" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J91" r:id="rId21" display="mailto:ALKHALIFAENTERPRISES@gmail.com" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J94" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:J16"/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="66" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="2.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="51.33203125" customWidth="1"/>
-    <col min="8" max="8" width="71.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" customWidth="1"/>
+    <col min="8" max="8" width="71.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="148" t="s">
         <v>1325</v>
       </c>
@@ -7031,7 +7067,7 @@
       <c r="I1" s="148"/>
       <c r="J1" s="148"/>
     </row>
-    <row r="2" spans="3:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="112" t="s">
         <v>693</v>
       </c>
@@ -7054,7 +7090,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="3" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="56">
         <v>1</v>
       </c>
@@ -7080,7 +7116,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="4" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="56">
         <v>2</v>
       </c>
@@ -7102,7 +7138,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="56">
         <v>3</v>
       </c>
@@ -7128,7 +7164,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="56">
         <v>4</v>
       </c>
@@ -7150,7 +7186,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="56">
         <v>5</v>
       </c>
@@ -7176,7 +7212,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="56">
         <v>6</v>
       </c>
@@ -7200,7 +7236,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="56">
         <v>7</v>
       </c>
@@ -7224,7 +7260,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="56">
         <v>8</v>
       </c>
@@ -7250,7 +7286,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="56">
         <v>9</v>
       </c>
@@ -7274,7 +7310,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="12" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="56">
         <v>10</v>
       </c>
@@ -7300,7 +7336,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="56">
         <v>11</v>
       </c>
@@ -7322,7 +7358,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="56">
         <v>12</v>
       </c>
@@ -7346,7 +7382,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="56">
         <v>13</v>
       </c>
@@ -7370,7 +7406,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="56">
         <v>14</v>
       </c>
@@ -7401,44 +7437,44 @@
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J14" r:id="rId1"/>
-    <hyperlink ref="J16" r:id="rId2"/>
-    <hyperlink ref="J7" r:id="rId3"/>
-    <hyperlink ref="J12" r:id="rId4"/>
-    <hyperlink ref="J3" r:id="rId5"/>
-    <hyperlink ref="J10" r:id="rId6"/>
-    <hyperlink ref="J4" r:id="rId7"/>
-    <hyperlink ref="J13" r:id="rId8"/>
-    <hyperlink ref="J6" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J15" r:id="rId11"/>
+    <hyperlink ref="J14" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="J7" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J12" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="J3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="J10" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="J4" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="J13" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="J6" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="J15" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="67" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="67" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" customWidth="1"/>
-    <col min="5" max="5" width="39.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="84" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" customWidth="1"/>
-    <col min="10" max="10" width="39.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="84" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" customWidth="1"/>
     <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
       <c r="E2" s="13" t="s">
@@ -7463,7 +7499,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="3" spans="3:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="18" t="s">
         <v>825</v>
       </c>
@@ -7476,7 +7512,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="15"/>
     </row>
-    <row r="4" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="97"/>
       <c r="D4" s="98">
         <v>1</v>
@@ -7499,7 +7535,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="5" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="79"/>
       <c r="D5" s="6">
         <v>2</v>
@@ -7522,7 +7558,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="79"/>
       <c r="D6" s="6">
         <v>3</v>
@@ -7545,7 +7581,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="79"/>
       <c r="D7" s="6">
         <v>4</v>
@@ -7568,7 +7604,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="8" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="21"/>
       <c r="D8" s="6">
         <v>5</v>
@@ -7591,7 +7627,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="6">
         <v>6</v>
@@ -7616,7 +7652,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="24"/>
       <c r="D10" s="6">
         <v>7</v>
@@ -7643,7 +7679,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="26"/>
       <c r="D11" s="6">
         <v>8</v>
@@ -7666,7 +7702,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="24"/>
       <c r="D12" s="6">
         <v>9</v>
@@ -7689,7 +7725,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="24"/>
       <c r="D13" s="6">
         <v>10</v>
@@ -7712,7 +7748,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="49"/>
       <c r="D14" s="6">
         <v>11</v>
@@ -7735,7 +7771,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="24"/>
       <c r="D15" s="6">
         <v>12</v>
@@ -7762,7 +7798,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="24"/>
       <c r="D16" s="6">
         <v>13</v>
@@ -7787,7 +7823,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="24"/>
       <c r="D17" s="6">
         <v>14</v>
@@ -7814,7 +7850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="24"/>
       <c r="D18" s="6">
         <v>15</v>
@@ -7841,7 +7877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="34"/>
       <c r="D19" s="6">
         <v>16</v>
@@ -7866,7 +7902,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="24"/>
       <c r="D20" s="6">
         <v>17</v>
@@ -7893,7 +7929,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="21" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="24"/>
       <c r="D21" s="6">
         <v>18</v>
@@ -7918,7 +7954,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="22" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="24"/>
       <c r="D22" s="6">
         <v>19</v>
@@ -7943,7 +7979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="26"/>
       <c r="D23" s="6">
         <v>20</v>
@@ -7966,7 +8002,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="24" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="24"/>
       <c r="D24" s="6">
         <v>21</v>
@@ -7991,7 +8027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="49"/>
       <c r="D25" s="6">
         <v>22</v>
@@ -8014,7 +8050,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="26" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="26"/>
       <c r="D26" s="6">
         <v>23</v>
@@ -8039,7 +8075,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="27" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="24"/>
       <c r="D27" s="6">
         <v>24</v>
@@ -8064,7 +8100,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="28" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="24"/>
       <c r="D28" s="6">
         <v>25</v>
@@ -8087,7 +8123,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="29" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="24"/>
       <c r="D29" s="6">
         <v>26</v>
@@ -8114,7 +8150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="24"/>
       <c r="D30" s="6">
         <v>27</v>
@@ -8139,7 +8175,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="31" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="24"/>
       <c r="D31" s="6">
         <v>28</v>
@@ -8162,7 +8198,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="24"/>
       <c r="D32" s="6">
         <v>29</v>
@@ -8185,7 +8221,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="33" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="24"/>
       <c r="D33" s="6">
         <v>30</v>
@@ -8210,7 +8246,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="34" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="26"/>
       <c r="D34" s="6">
         <v>31</v>
@@ -8233,7 +8269,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="35" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="26"/>
       <c r="D35" s="6">
         <v>32</v>
@@ -8256,7 +8292,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="36" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="24"/>
       <c r="D36" s="6">
         <v>33</v>
@@ -8283,7 +8319,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="24"/>
       <c r="D37" s="6">
         <v>34</v>
@@ -8308,7 +8344,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="49"/>
       <c r="D38" s="6">
         <v>35</v>
@@ -8331,7 +8367,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="39" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="24"/>
       <c r="D39" s="6">
         <v>36</v>
@@ -8358,7 +8394,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="24"/>
       <c r="D40" s="6">
         <v>37</v>
@@ -8385,7 +8421,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="41" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="24"/>
       <c r="D41" s="6">
         <v>38</v>
@@ -8412,7 +8448,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="24"/>
       <c r="D42" s="6">
         <v>39</v>
@@ -8439,7 +8475,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="43" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="26"/>
       <c r="D43" s="6">
         <v>40</v>
@@ -8464,7 +8500,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="44" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="104"/>
       <c r="D44" s="98">
         <v>41</v>
@@ -8487,7 +8523,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="45" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="104"/>
       <c r="D45" s="98">
         <v>42</v>
@@ -8510,7 +8546,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="46" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="104"/>
       <c r="D46" s="98">
         <v>43</v>
@@ -8533,7 +8569,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="47" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="24"/>
       <c r="D47" s="6">
         <v>44</v>
@@ -8560,7 +8596,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="48" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="43"/>
       <c r="D48" s="6">
         <v>45</v>
@@ -8587,7 +8623,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="49" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="18" t="s">
         <v>64</v>
       </c>
@@ -8614,7 +8650,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="50" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="44"/>
       <c r="D50" s="6">
         <v>47</v>
@@ -8637,7 +8673,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="51" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="46"/>
       <c r="D51" s="6">
         <v>48</v>
@@ -8662,7 +8698,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="52" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="26"/>
       <c r="D52" s="6">
         <v>49</v>
@@ -8689,7 +8725,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="26"/>
       <c r="D53" s="6">
         <v>50</v>
@@ -8712,7 +8748,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="54" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="24"/>
       <c r="D54" s="6">
         <v>51</v>
@@ -8737,7 +8773,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="24"/>
       <c r="D55" s="6">
         <v>52</v>
@@ -8762,7 +8798,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="24"/>
       <c r="D56" s="6">
         <v>53</v>
@@ -8785,7 +8821,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="57" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="24"/>
       <c r="D57" s="6">
         <v>54</v>
@@ -8810,7 +8846,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="24"/>
       <c r="D58" s="6">
         <v>55</v>
@@ -8833,7 +8869,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="24"/>
       <c r="D59" s="6">
         <v>56</v>
@@ -8858,7 +8894,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="60" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="24"/>
       <c r="D60" s="6">
         <v>57</v>
@@ -8883,7 +8919,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="24"/>
       <c r="D61" s="6">
         <v>58</v>
@@ -8908,7 +8944,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="62" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="24"/>
       <c r="D62" s="6">
         <v>59</v>
@@ -8933,7 +8969,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="63" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="24"/>
       <c r="D63" s="6">
         <v>60</v>
@@ -8958,7 +8994,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="64" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="48"/>
       <c r="D64" s="6">
         <v>61</v>
@@ -8983,7 +9019,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="65" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="24"/>
       <c r="D65" s="6">
         <v>62</v>
@@ -9010,7 +9046,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="24"/>
       <c r="D66" s="6">
         <v>63</v>
@@ -9033,7 +9069,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="67" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="24"/>
       <c r="D67" s="6">
         <v>64</v>
@@ -9060,7 +9096,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="18" t="s">
         <v>113</v>
       </c>
@@ -9087,7 +9123,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="49"/>
       <c r="D69" s="6">
         <v>66</v>
@@ -9114,7 +9150,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="49"/>
       <c r="D70" s="6">
         <v>67</v>
@@ -9139,7 +9175,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="49"/>
       <c r="D71" s="6">
         <v>68</v>
@@ -9164,7 +9200,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="72" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="49"/>
       <c r="D72" s="6">
         <v>69</v>
@@ -9189,7 +9225,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="73" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="49"/>
       <c r="D73" s="6">
         <v>70</v>
@@ -9214,7 +9250,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="2"/>
       <c r="D74" s="6">
         <v>71</v>
@@ -9239,7 +9275,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="75" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="18" t="s">
         <v>132</v>
       </c>
@@ -9264,7 +9300,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="76" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="2"/>
       <c r="D76" s="6">
         <v>73</v>
@@ -9289,7 +9325,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="77" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="2"/>
       <c r="D77" s="6">
         <v>74</v>
@@ -9314,7 +9350,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="78" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="24"/>
       <c r="D78" s="6">
         <v>75</v>
@@ -9339,7 +9375,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="79" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="24"/>
       <c r="D79" s="6">
         <v>76</v>
@@ -9366,7 +9402,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="80" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="24"/>
       <c r="D80" s="6">
         <v>77</v>
@@ -9391,7 +9427,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="81" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="2"/>
       <c r="D81" s="6">
         <v>78</v>
@@ -9414,7 +9450,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="82" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="24"/>
       <c r="D82" s="6">
         <v>79</v>
@@ -9439,7 +9475,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="83" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="24"/>
       <c r="D83" s="6">
         <v>80</v>
@@ -9464,7 +9500,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="84" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="24"/>
       <c r="D84" s="6">
         <v>81</v>
@@ -9491,7 +9527,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="24"/>
       <c r="D85" s="6">
         <v>82</v>
@@ -9514,7 +9550,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="86" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="24"/>
       <c r="D86" s="6">
         <v>83</v>
@@ -9539,7 +9575,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="87" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="18" t="s">
         <v>143</v>
       </c>
@@ -9568,7 +9604,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="88" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="24"/>
       <c r="D88" s="6">
         <v>85</v>
@@ -9593,7 +9629,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="89" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="53" t="s">
         <v>152</v>
       </c>
@@ -9620,7 +9656,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="24"/>
       <c r="D90" s="6">
         <v>87</v>
@@ -9643,7 +9679,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="91" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="18" t="s">
         <v>157</v>
       </c>
@@ -9670,7 +9706,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="49"/>
       <c r="D92" s="6">
         <v>89</v>
@@ -9695,7 +9731,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="18" t="s">
         <v>470</v>
       </c>
@@ -9722,7 +9758,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="94" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="18" t="s">
         <v>170</v>
       </c>
@@ -9749,7 +9785,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="95" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="2"/>
       <c r="D95" s="6">
         <v>92</v>
@@ -9776,7 +9812,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="96" spans="3:11" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="18" t="s">
         <v>872</v>
       </c>
@@ -9805,88 +9841,88 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K58" r:id="rId1"/>
-    <hyperlink ref="K69" r:id="rId2"/>
-    <hyperlink ref="K62" r:id="rId3"/>
-    <hyperlink ref="K86" r:id="rId4"/>
-    <hyperlink ref="K68" r:id="rId5"/>
-    <hyperlink ref="K67" r:id="rId6"/>
-    <hyperlink ref="K54" r:id="rId7" display="kijuratea@yahoo.com"/>
-    <hyperlink ref="K65" r:id="rId8"/>
-    <hyperlink ref="K84" r:id="rId9"/>
-    <hyperlink ref="K57" r:id="rId10"/>
-    <hyperlink ref="K55" r:id="rId11"/>
-    <hyperlink ref="K60" r:id="rId12"/>
-    <hyperlink ref="K88" r:id="rId13"/>
-    <hyperlink ref="K91" r:id="rId14"/>
-    <hyperlink ref="K52" r:id="rId15"/>
-    <hyperlink ref="K73" r:id="rId16"/>
-    <hyperlink ref="K92" r:id="rId17"/>
-    <hyperlink ref="K48" r:id="rId18"/>
-    <hyperlink ref="K21" r:id="rId19"/>
-    <hyperlink ref="K12" r:id="rId20"/>
-    <hyperlink ref="K30" r:id="rId21"/>
-    <hyperlink ref="K9" r:id="rId22" display="mailto:moses@thedlgroup.com"/>
-    <hyperlink ref="K49" r:id="rId23"/>
-    <hyperlink ref="K17" r:id="rId24"/>
-    <hyperlink ref="K16" r:id="rId25"/>
-    <hyperlink ref="K41" r:id="rId26"/>
-    <hyperlink ref="K10" r:id="rId27"/>
-    <hyperlink ref="K39" r:id="rId28"/>
-    <hyperlink ref="K18" r:id="rId29"/>
-    <hyperlink ref="K36" r:id="rId30"/>
-    <hyperlink ref="K33" r:id="rId31"/>
-    <hyperlink ref="K22" r:id="rId32"/>
-    <hyperlink ref="K29" r:id="rId33"/>
-    <hyperlink ref="K24" r:id="rId34"/>
-    <hyperlink ref="K27" r:id="rId35"/>
-    <hyperlink ref="K66" r:id="rId36"/>
-    <hyperlink ref="K94" r:id="rId37"/>
-    <hyperlink ref="K56" r:id="rId38"/>
-    <hyperlink ref="K61" r:id="rId39" display="mailto:nyambya@gmail.com"/>
-    <hyperlink ref="K82" r:id="rId40"/>
-    <hyperlink ref="K59" r:id="rId41" display="mailto:gm.tea@madhvanitea.co.ug"/>
-    <hyperlink ref="K26" r:id="rId42"/>
-    <hyperlink ref="K50" r:id="rId43"/>
-    <hyperlink ref="K90" r:id="rId44"/>
-    <hyperlink ref="K96" r:id="rId45"/>
-    <hyperlink ref="K35" r:id="rId46"/>
-    <hyperlink ref="K4" r:id="rId47"/>
-    <hyperlink ref="K11" r:id="rId48"/>
-    <hyperlink ref="K76" r:id="rId49"/>
-    <hyperlink ref="K77" r:id="rId50"/>
-    <hyperlink ref="K74" r:id="rId51"/>
-    <hyperlink ref="K78" r:id="rId52"/>
-    <hyperlink ref="K40" r:id="rId53"/>
-    <hyperlink ref="K85" r:id="rId54"/>
-    <hyperlink ref="K81" r:id="rId55"/>
-    <hyperlink ref="K13" r:id="rId56"/>
-    <hyperlink ref="K43" r:id="rId57"/>
-    <hyperlink ref="K51" r:id="rId58"/>
-    <hyperlink ref="K64" r:id="rId59"/>
-    <hyperlink ref="K34" r:id="rId60"/>
-    <hyperlink ref="K72" r:id="rId61"/>
-    <hyperlink ref="K70" r:id="rId62"/>
-    <hyperlink ref="K31" r:id="rId63"/>
-    <hyperlink ref="K89" r:id="rId64"/>
-    <hyperlink ref="K20" r:id="rId65"/>
-    <hyperlink ref="K53" r:id="rId66"/>
-    <hyperlink ref="K45" r:id="rId67"/>
-    <hyperlink ref="K28" r:id="rId68"/>
-    <hyperlink ref="K8" r:id="rId69"/>
-    <hyperlink ref="K93" r:id="rId70"/>
-    <hyperlink ref="K38" r:id="rId71"/>
-    <hyperlink ref="K14" r:id="rId72"/>
-    <hyperlink ref="K23" r:id="rId73"/>
-    <hyperlink ref="K7" r:id="rId74"/>
-    <hyperlink ref="K25" r:id="rId75"/>
-    <hyperlink ref="K75" r:id="rId76"/>
-    <hyperlink ref="K32" r:id="rId77"/>
-    <hyperlink ref="K37" r:id="rId78"/>
-    <hyperlink ref="K6" r:id="rId79"/>
-    <hyperlink ref="K83" r:id="rId80"/>
-    <hyperlink ref="K46" r:id="rId81"/>
-    <hyperlink ref="K44" r:id="rId82"/>
+    <hyperlink ref="K58" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="K69" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="K62" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="K86" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="K68" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="K67" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="K54" r:id="rId7" display="kijuratea@yahoo.com" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="K65" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="K84" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="K57" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="K55" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="K60" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="K88" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="K91" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="K52" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="K73" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="K92" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="K48" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="K21" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="K12" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="K30" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="K9" r:id="rId22" display="mailto:moses@thedlgroup.com" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="K49" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="K17" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="K16" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="K41" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="K10" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="K39" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="K18" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="K36" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="K33" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="K22" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="K29" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="K24" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="K27" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="K66" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="K94" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="K56" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="K61" r:id="rId39" display="mailto:nyambya@gmail.com" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="K82" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="K59" r:id="rId41" display="mailto:gm.tea@madhvanitea.co.ug" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="K26" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="K50" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="K90" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="K96" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="K35" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="K4" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="K11" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="K76" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="K77" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="K74" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="K78" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="K40" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="K85" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="K81" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="K13" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="K43" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="K51" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="K64" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="K34" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="K72" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="K70" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="K31" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="K89" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="K20" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="K53" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="K45" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="K28" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="K8" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="K93" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="K38" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="K14" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="K23" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="K7" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="K25" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="K75" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="K32" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="K37" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="K6" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="K83" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="K46" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="K44" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId83"/>
@@ -9894,26 +9930,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:J97"/>
   <sheetViews>
     <sheetView topLeftCell="A88" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N88" sqref="N88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="43.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="43.6640625" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" customWidth="1"/>
-    <col min="9" max="9" width="47.21875" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" customWidth="1"/>
+    <col min="9" max="9" width="47.28515625" customWidth="1"/>
     <col min="10" max="10" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="148" t="s">
         <v>1324</v>
       </c>
@@ -9925,7 +9961,7 @@
       <c r="I1" s="148"/>
       <c r="J1" s="148"/>
     </row>
-    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="112" t="s">
         <v>693</v>
       </c>
@@ -9948,7 +9984,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="113">
         <v>1</v>
       </c>
@@ -9972,7 +10008,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="113">
         <v>2</v>
       </c>
@@ -9996,7 +10032,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="113">
         <v>3</v>
       </c>
@@ -10020,7 +10056,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="113">
         <v>4</v>
@@ -10045,7 +10081,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="113">
         <v>5</v>
       </c>
@@ -10067,7 +10103,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="113">
         <v>6</v>
       </c>
@@ -10091,7 +10127,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="113">
         <v>7</v>
       </c>
@@ -10113,7 +10149,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="113">
         <v>8</v>
       </c>
@@ -10135,7 +10171,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="113">
         <v>9</v>
       </c>
@@ -10161,7 +10197,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="113">
         <v>10</v>
       </c>
@@ -10187,7 +10223,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="113">
         <v>11</v>
       </c>
@@ -10211,7 +10247,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="113">
         <v>12</v>
       </c>
@@ -10235,7 +10271,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="115">
         <v>13</v>
       </c>
@@ -10257,7 +10293,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="113">
         <v>14</v>
       </c>
@@ -10281,7 +10317,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="113">
         <v>15</v>
       </c>
@@ -10307,7 +10343,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="113">
         <v>16</v>
       </c>
@@ -10331,7 +10367,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="113">
         <v>17</v>
       </c>
@@ -10353,7 +10389,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="113">
         <v>18</v>
       </c>
@@ -10377,7 +10413,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="113">
         <v>19</v>
       </c>
@@ -10403,7 +10439,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="113">
         <v>20</v>
       </c>
@@ -10425,7 +10461,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="23" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="113">
         <v>21</v>
       </c>
@@ -10449,7 +10485,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="113">
         <v>22</v>
       </c>
@@ -10473,7 +10509,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="113">
         <v>23</v>
       </c>
@@ -10495,7 +10531,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="113">
         <v>24</v>
       </c>
@@ -10519,7 +10555,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="27" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="113">
         <v>25</v>
       </c>
@@ -10541,7 +10577,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="28" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="113">
         <v>26</v>
       </c>
@@ -10567,7 +10603,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="113">
         <v>27</v>
       </c>
@@ -10591,7 +10627,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="30" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="113">
         <v>28</v>
       </c>
@@ -10615,7 +10651,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="31" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="113">
         <v>29</v>
       </c>
@@ -10639,7 +10675,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="32" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="113">
         <v>30</v>
       </c>
@@ -10661,7 +10697,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="113">
         <v>31</v>
       </c>
@@ -10685,7 +10721,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="115">
         <v>32</v>
       </c>
@@ -10707,7 +10743,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="115">
         <v>33</v>
       </c>
@@ -10729,7 +10765,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="113">
         <v>34</v>
       </c>
@@ -10755,7 +10791,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="37" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="113">
         <v>35</v>
       </c>
@@ -10781,7 +10817,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="38" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="113">
         <v>36</v>
       </c>
@@ -10803,7 +10839,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="39" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="113">
         <v>37</v>
       </c>
@@ -10827,7 +10863,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="40" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="113">
         <v>38</v>
       </c>
@@ -10849,7 +10885,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="41" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="113">
         <v>39</v>
       </c>
@@ -10871,7 +10907,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="42" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="113">
         <v>40</v>
       </c>
@@ -10893,7 +10929,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="43" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="113">
         <v>41</v>
       </c>
@@ -10917,7 +10953,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="113">
         <v>42</v>
       </c>
@@ -10939,7 +10975,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="113">
         <v>43</v>
       </c>
@@ -10963,7 +10999,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="46" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="113">
         <v>44</v>
       </c>
@@ -10987,7 +11023,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="47" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="113">
         <v>45</v>
       </c>
@@ -11009,7 +11045,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="48" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="113">
         <v>46</v>
       </c>
@@ -11033,7 +11069,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="113">
         <v>47</v>
       </c>
@@ -11057,7 +11093,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="113">
         <v>48</v>
       </c>
@@ -11081,7 +11117,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="113">
         <v>49</v>
       </c>
@@ -11105,7 +11141,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="52" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="113">
         <v>50</v>
       </c>
@@ -11127,7 +11163,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="53" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="113">
         <v>51</v>
       </c>
@@ -11151,7 +11187,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="54" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="113">
         <v>52</v>
       </c>
@@ -11173,7 +11209,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="55" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="113">
         <v>53</v>
       </c>
@@ -11197,7 +11233,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="56" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="113">
         <v>54</v>
       </c>
@@ -11223,7 +11259,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="57" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="113">
         <v>55</v>
       </c>
@@ -11247,7 +11283,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="58" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="113">
         <v>56</v>
       </c>
@@ -11273,7 +11309,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="59" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="113">
         <v>57</v>
       </c>
@@ -11299,7 +11335,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="60" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="113">
         <v>58</v>
       </c>
@@ -11321,7 +11357,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="61" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="113">
         <v>59</v>
       </c>
@@ -11343,7 +11379,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="62" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="113">
         <v>60</v>
       </c>
@@ -11365,7 +11401,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="63" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="113">
         <v>61</v>
       </c>
@@ -11389,7 +11425,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="113">
         <v>62</v>
       </c>
@@ -11415,7 +11451,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="65" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="113">
         <v>63</v>
       </c>
@@ -11441,7 +11477,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="66" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="113">
         <v>64</v>
       </c>
@@ -11467,7 +11503,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="67" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="113">
         <v>65</v>
       </c>
@@ -11489,7 +11525,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="68" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="113">
         <v>66</v>
       </c>
@@ -11511,7 +11547,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="69" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="113">
         <v>67</v>
       </c>
@@ -11533,7 +11569,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="70" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="113">
         <v>68</v>
       </c>
@@ -11557,7 +11593,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="71" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="113">
         <v>69</v>
       </c>
@@ -11583,7 +11619,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="72" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="113">
         <v>70</v>
       </c>
@@ -11607,7 +11643,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="73" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="113">
         <v>71</v>
       </c>
@@ -11631,7 +11667,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="74" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="113">
         <v>72</v>
       </c>
@@ -11653,7 +11689,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="75" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="113">
         <v>73</v>
       </c>
@@ -11677,7 +11713,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="76" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="113">
         <v>74</v>
       </c>
@@ -11703,7 +11739,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="77" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="113">
         <v>75</v>
       </c>
@@ -11725,7 +11761,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="78" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="113">
         <v>76</v>
       </c>
@@ -11751,7 +11787,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="79" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="113">
         <v>77</v>
       </c>
@@ -11775,7 +11811,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="80" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="113">
         <v>78</v>
       </c>
@@ -11799,7 +11835,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="81" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="113">
         <v>79</v>
       </c>
@@ -11823,7 +11859,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="82" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="113">
         <v>80</v>
       </c>
@@ -11849,7 +11885,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="83" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="113">
         <v>81</v>
       </c>
@@ -11873,7 +11909,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="84" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="113">
         <v>82</v>
       </c>
@@ -11897,7 +11933,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="85" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="113">
         <v>83</v>
       </c>
@@ -11919,7 +11955,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="86" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="113">
         <v>84</v>
       </c>
@@ -11941,7 +11977,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="87" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="113">
         <v>85</v>
       </c>
@@ -11963,7 +11999,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="88" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="113">
         <v>86</v>
       </c>
@@ -11985,7 +12021,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="89" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="113">
         <v>87</v>
       </c>
@@ -12007,7 +12043,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="90" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="113">
         <v>88</v>
       </c>
@@ -12029,7 +12065,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="91" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="113">
         <v>89</v>
       </c>
@@ -12051,7 +12087,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="92" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="113">
         <v>90</v>
       </c>
@@ -12073,7 +12109,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="93" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="113">
         <v>91</v>
       </c>
@@ -12097,7 +12133,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="94" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="113">
         <v>92</v>
       </c>
@@ -12119,7 +12155,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="95" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="113">
         <v>93</v>
       </c>
@@ -12143,7 +12179,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="96" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="113">
         <v>94</v>
       </c>
@@ -12169,7 +12205,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="97" spans="3:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="113">
         <v>95</v>
       </c>
@@ -12196,96 +12232,96 @@
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
-    <hyperlink ref="J96" r:id="rId2"/>
-    <hyperlink ref="J12" r:id="rId3"/>
-    <hyperlink ref="J23" r:id="rId4"/>
-    <hyperlink ref="J48" r:id="rId5"/>
-    <hyperlink ref="J79" r:id="rId6"/>
-    <hyperlink ref="J24" r:id="rId7"/>
-    <hyperlink ref="J93" r:id="rId8"/>
-    <hyperlink ref="J71" r:id="rId9"/>
-    <hyperlink ref="J78" r:id="rId10"/>
-    <hyperlink ref="J66" r:id="rId11"/>
-    <hyperlink ref="J5" r:id="rId12"/>
-    <hyperlink ref="J11" r:id="rId13"/>
-    <hyperlink ref="J20" r:id="rId14"/>
-    <hyperlink ref="J75" r:id="rId15"/>
-    <hyperlink ref="J72" r:id="rId16"/>
-    <hyperlink ref="J21" r:id="rId17" display="chamutradingtea@yahoo.com"/>
-    <hyperlink ref="J14" r:id="rId18" display="apttea@yahoo.com"/>
-    <hyperlink ref="J6" r:id="rId19" display="atc@africaonline.co.ke"/>
-    <hyperlink ref="J50" r:id="rId20"/>
-    <hyperlink ref="J18" r:id="rId21"/>
-    <hyperlink ref="J43" r:id="rId22"/>
-    <hyperlink ref="J52" r:id="rId23" display="info@kenyanut.com"/>
-    <hyperlink ref="J65" r:id="rId24"/>
-    <hyperlink ref="J53" r:id="rId25"/>
-    <hyperlink ref="J56" r:id="rId26"/>
-    <hyperlink ref="J57" r:id="rId27"/>
-    <hyperlink ref="J55" r:id="rId28"/>
-    <hyperlink ref="J58" r:id="rId29"/>
-    <hyperlink ref="J7" r:id="rId30"/>
-    <hyperlink ref="J40" r:id="rId31"/>
-    <hyperlink ref="J92" r:id="rId32"/>
-    <hyperlink ref="J97" r:id="rId33"/>
-    <hyperlink ref="J82" r:id="rId34"/>
-    <hyperlink ref="J83" r:id="rId35"/>
-    <hyperlink ref="J10" r:id="rId36" display="mailto:ALKHALIFAENTERPRISES@gmail.com"/>
-    <hyperlink ref="J8" r:id="rId37"/>
-    <hyperlink ref="J19" r:id="rId38"/>
-    <hyperlink ref="J13" r:id="rId39" display="mailto:alitihadltd@yahoo.com"/>
-    <hyperlink ref="J80" r:id="rId40"/>
-    <hyperlink ref="J62" r:id="rId41"/>
-    <hyperlink ref="J16" r:id="rId42"/>
-    <hyperlink ref="J90" r:id="rId43"/>
-    <hyperlink ref="J26" r:id="rId44"/>
-    <hyperlink ref="J17" r:id="rId45"/>
-    <hyperlink ref="J95" r:id="rId46"/>
-    <hyperlink ref="J85" r:id="rId47"/>
-    <hyperlink ref="J29" r:id="rId48"/>
-    <hyperlink ref="J49" r:id="rId49"/>
-    <hyperlink ref="J9" r:id="rId50"/>
-    <hyperlink ref="J73" r:id="rId51"/>
-    <hyperlink ref="J76" r:id="rId52"/>
-    <hyperlink ref="J25" r:id="rId53"/>
-    <hyperlink ref="J31" r:id="rId54"/>
-    <hyperlink ref="J45" r:id="rId55"/>
-    <hyperlink ref="J64" r:id="rId56"/>
-    <hyperlink ref="J69" r:id="rId57"/>
-    <hyperlink ref="J94" r:id="rId58"/>
-    <hyperlink ref="J86" r:id="rId59"/>
-    <hyperlink ref="J87" r:id="rId60"/>
-    <hyperlink ref="J84" r:id="rId61"/>
-    <hyperlink ref="J77" r:id="rId62"/>
-    <hyperlink ref="J91" r:id="rId63"/>
-    <hyperlink ref="J46" r:id="rId64"/>
-    <hyperlink ref="J39" r:id="rId65"/>
-    <hyperlink ref="J42" r:id="rId66"/>
-    <hyperlink ref="J88" r:id="rId67"/>
-    <hyperlink ref="J27" r:id="rId68" display="nobahar@delstatea.com"/>
-    <hyperlink ref="J61" r:id="rId69"/>
-    <hyperlink ref="J47" r:id="rId70"/>
-    <hyperlink ref="J28" r:id="rId71"/>
-    <hyperlink ref="J32" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J38" r:id="rId74"/>
-    <hyperlink ref="J44" r:id="rId75"/>
-    <hyperlink ref="J68" r:id="rId76"/>
-    <hyperlink ref="J22" r:id="rId77" display="mailto:info@classictea.co.ke"/>
-    <hyperlink ref="J54" r:id="rId78"/>
-    <hyperlink ref="J60" r:id="rId79"/>
-    <hyperlink ref="J67" r:id="rId80"/>
-    <hyperlink ref="J41" r:id="rId81"/>
-    <hyperlink ref="J30" r:id="rId82"/>
-    <hyperlink ref="J89" r:id="rId83"/>
-    <hyperlink ref="J4" r:id="rId84"/>
-    <hyperlink ref="J36" r:id="rId85"/>
-    <hyperlink ref="J37" r:id="rId86"/>
-    <hyperlink ref="J33" r:id="rId87"/>
-    <hyperlink ref="J15" r:id="rId88"/>
-    <hyperlink ref="J34" r:id="rId89"/>
-    <hyperlink ref="J35" r:id="rId90"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="J96" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="J12" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="J23" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="J48" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="J79" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="J24" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="J93" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="J71" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="J78" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="J66" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="J5" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="J11" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="J20" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="J75" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="J72" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="J21" r:id="rId17" display="chamutradingtea@yahoo.com" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="J14" r:id="rId18" display="apttea@yahoo.com" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="J6" r:id="rId19" display="atc@africaonline.co.ke" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="J50" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="J18" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="J43" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="J52" r:id="rId23" display="info@kenyanut.com" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
+    <hyperlink ref="J65" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
+    <hyperlink ref="J53" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
+    <hyperlink ref="J56" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
+    <hyperlink ref="J57" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
+    <hyperlink ref="J55" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
+    <hyperlink ref="J58" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
+    <hyperlink ref="J7" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
+    <hyperlink ref="J40" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
+    <hyperlink ref="J92" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
+    <hyperlink ref="J97" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
+    <hyperlink ref="J82" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
+    <hyperlink ref="J83" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
+    <hyperlink ref="J10" r:id="rId36" display="mailto:ALKHALIFAENTERPRISES@gmail.com" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
+    <hyperlink ref="J8" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
+    <hyperlink ref="J19" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
+    <hyperlink ref="J13" r:id="rId39" display="mailto:alitihadltd@yahoo.com" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
+    <hyperlink ref="J80" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
+    <hyperlink ref="J62" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
+    <hyperlink ref="J16" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
+    <hyperlink ref="J90" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
+    <hyperlink ref="J26" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
+    <hyperlink ref="J17" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
+    <hyperlink ref="J95" r:id="rId46" xr:uid="{00000000-0004-0000-0300-00002D000000}"/>
+    <hyperlink ref="J85" r:id="rId47" xr:uid="{00000000-0004-0000-0300-00002E000000}"/>
+    <hyperlink ref="J29" r:id="rId48" xr:uid="{00000000-0004-0000-0300-00002F000000}"/>
+    <hyperlink ref="J49" r:id="rId49" xr:uid="{00000000-0004-0000-0300-000030000000}"/>
+    <hyperlink ref="J9" r:id="rId50" xr:uid="{00000000-0004-0000-0300-000031000000}"/>
+    <hyperlink ref="J73" r:id="rId51" xr:uid="{00000000-0004-0000-0300-000032000000}"/>
+    <hyperlink ref="J76" r:id="rId52" xr:uid="{00000000-0004-0000-0300-000033000000}"/>
+    <hyperlink ref="J25" r:id="rId53" xr:uid="{00000000-0004-0000-0300-000034000000}"/>
+    <hyperlink ref="J31" r:id="rId54" xr:uid="{00000000-0004-0000-0300-000035000000}"/>
+    <hyperlink ref="J45" r:id="rId55" xr:uid="{00000000-0004-0000-0300-000036000000}"/>
+    <hyperlink ref="J64" r:id="rId56" xr:uid="{00000000-0004-0000-0300-000037000000}"/>
+    <hyperlink ref="J69" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000038000000}"/>
+    <hyperlink ref="J94" r:id="rId58" xr:uid="{00000000-0004-0000-0300-000039000000}"/>
+    <hyperlink ref="J86" r:id="rId59" xr:uid="{00000000-0004-0000-0300-00003A000000}"/>
+    <hyperlink ref="J87" r:id="rId60" xr:uid="{00000000-0004-0000-0300-00003B000000}"/>
+    <hyperlink ref="J84" r:id="rId61" xr:uid="{00000000-0004-0000-0300-00003C000000}"/>
+    <hyperlink ref="J77" r:id="rId62" xr:uid="{00000000-0004-0000-0300-00003D000000}"/>
+    <hyperlink ref="J91" r:id="rId63" xr:uid="{00000000-0004-0000-0300-00003E000000}"/>
+    <hyperlink ref="J46" r:id="rId64" xr:uid="{00000000-0004-0000-0300-00003F000000}"/>
+    <hyperlink ref="J39" r:id="rId65" xr:uid="{00000000-0004-0000-0300-000040000000}"/>
+    <hyperlink ref="J42" r:id="rId66" xr:uid="{00000000-0004-0000-0300-000041000000}"/>
+    <hyperlink ref="J88" r:id="rId67" xr:uid="{00000000-0004-0000-0300-000042000000}"/>
+    <hyperlink ref="J27" r:id="rId68" display="nobahar@delstatea.com" xr:uid="{00000000-0004-0000-0300-000043000000}"/>
+    <hyperlink ref="J61" r:id="rId69" xr:uid="{00000000-0004-0000-0300-000044000000}"/>
+    <hyperlink ref="J47" r:id="rId70" xr:uid="{00000000-0004-0000-0300-000045000000}"/>
+    <hyperlink ref="J28" r:id="rId71" xr:uid="{00000000-0004-0000-0300-000046000000}"/>
+    <hyperlink ref="J32" r:id="rId72" xr:uid="{00000000-0004-0000-0300-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0300-000048000000}"/>
+    <hyperlink ref="J38" r:id="rId74" xr:uid="{00000000-0004-0000-0300-000049000000}"/>
+    <hyperlink ref="J44" r:id="rId75" xr:uid="{00000000-0004-0000-0300-00004A000000}"/>
+    <hyperlink ref="J68" r:id="rId76" xr:uid="{00000000-0004-0000-0300-00004B000000}"/>
+    <hyperlink ref="J22" r:id="rId77" display="mailto:info@classictea.co.ke" xr:uid="{00000000-0004-0000-0300-00004C000000}"/>
+    <hyperlink ref="J54" r:id="rId78" xr:uid="{00000000-0004-0000-0300-00004D000000}"/>
+    <hyperlink ref="J60" r:id="rId79" xr:uid="{00000000-0004-0000-0300-00004E000000}"/>
+    <hyperlink ref="J67" r:id="rId80" xr:uid="{00000000-0004-0000-0300-00004F000000}"/>
+    <hyperlink ref="J41" r:id="rId81" xr:uid="{00000000-0004-0000-0300-000050000000}"/>
+    <hyperlink ref="J30" r:id="rId82" xr:uid="{00000000-0004-0000-0300-000051000000}"/>
+    <hyperlink ref="J89" r:id="rId83" xr:uid="{00000000-0004-0000-0300-000052000000}"/>
+    <hyperlink ref="J4" r:id="rId84" xr:uid="{00000000-0004-0000-0300-000053000000}"/>
+    <hyperlink ref="J36" r:id="rId85" xr:uid="{00000000-0004-0000-0300-000054000000}"/>
+    <hyperlink ref="J37" r:id="rId86" xr:uid="{00000000-0004-0000-0300-000055000000}"/>
+    <hyperlink ref="J33" r:id="rId87" xr:uid="{00000000-0004-0000-0300-000056000000}"/>
+    <hyperlink ref="J15" r:id="rId88" xr:uid="{00000000-0004-0000-0300-000057000000}"/>
+    <hyperlink ref="J34" r:id="rId89" xr:uid="{00000000-0004-0000-0300-000058000000}"/>
+    <hyperlink ref="J35" r:id="rId90" xr:uid="{00000000-0004-0000-0300-000059000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="296" orientation="portrait" r:id="rId91"/>
@@ -12293,23 +12329,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="D3:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="6.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="148" t="s">
         <v>1327</v>
       </c>
@@ -12321,7 +12357,7 @@
       </c>
       <c r="K3" s="151"/>
     </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D4" s="149" t="s">
         <v>1328</v>
       </c>
@@ -12331,7 +12367,7 @@
       <c r="J4" s="149"/>
       <c r="K4" s="149"/>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="142"/>
       <c r="E5" s="142" t="s">
         <v>1343</v>
@@ -12347,7 +12383,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="144">
         <v>1</v>
       </c>
@@ -12367,7 +12403,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="144">
         <v>2</v>
       </c>
@@ -12387,7 +12423,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="144">
         <v>3</v>
       </c>
@@ -12407,7 +12443,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="144">
         <v>4</v>
       </c>
@@ -12427,7 +12463,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="144"/>
       <c r="E10" s="144"/>
       <c r="F10" s="145"/>
@@ -12439,7 +12475,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="149" t="s">
         <v>1333</v>
       </c>
@@ -12453,7 +12489,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="144">
         <v>1</v>
       </c>
@@ -12473,7 +12509,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="144">
         <v>2</v>
       </c>
@@ -12493,7 +12529,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="144">
         <v>3</v>
       </c>
@@ -12513,7 +12549,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="144">
         <v>4</v>
       </c>
@@ -12533,7 +12569,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="144">
         <v>5</v>
       </c>
@@ -12553,7 +12589,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="144">
         <v>6</v>
       </c>
@@ -12573,7 +12609,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="144">
         <v>7</v>
       </c>
@@ -12593,7 +12629,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="144">
         <v>8</v>
       </c>
@@ -12613,7 +12649,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="144">
         <v>9</v>
       </c>
@@ -12633,7 +12669,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="145"/>
       <c r="E21" s="145"/>
       <c r="F21" s="145"/>
@@ -12645,7 +12681,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J22" s="147">
         <v>17</v>
       </c>
@@ -12653,7 +12689,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J23" s="147">
         <v>18</v>
       </c>
@@ -12661,7 +12697,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J24" s="147">
         <v>19</v>
       </c>
@@ -12669,7 +12705,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J25" s="147">
         <v>20</v>
       </c>

</xml_diff>